<commit_message>
Old files delete, jangseong sql file correction
</commit_message>
<xml_diff>
--- a/jangseong/DataImport.xlsx
+++ b/jangseong/DataImport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\jangseong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\jangseong\jangseong\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D9200-58C7-4F29-A0D7-4B6A1835A013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27975" windowHeight="8085"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,51 +25,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>김원수</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+  <si>
+    <t>23-01</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>울산</t>
-  </si>
-  <si>
-    <t>김하은</t>
-  </si>
-  <si>
-    <t>김동연</t>
-  </si>
-  <si>
-    <t>23-123146</t>
-  </si>
-  <si>
-    <t>23-123137</t>
-  </si>
-  <si>
-    <t>23-3</t>
-  </si>
-  <si>
-    <t>23-12314</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>김채원</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>허윤진</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍은채</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>23-000001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>23-000002</t>
+  </si>
+  <si>
+    <t>23-000003</t>
+  </si>
+  <si>
+    <t>23-02</t>
+  </si>
+  <si>
+    <t>23-000004</t>
   </si>
   <si>
     <t>23-03</t>
   </si>
   <si>
-    <t>23-04</t>
+    <t>23-000005</t>
+  </si>
+  <si>
+    <t>카즈하</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사쿠라</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -76,14 +96,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -126,19 +146,28 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,77 +478,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="9" style="3"/>
+    <col min="2" max="2" width="9" style="4"/>
+    <col min="3" max="3" width="9" style="3"/>
+    <col min="4" max="4" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="5">
         <v>45213</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>45213</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>44999</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45000</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45001</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>